<commit_message>
Documents and auxiliary files
</commit_message>
<xml_diff>
--- a/doc/INF1.paper.xlsx
+++ b/doc/INF1.paper.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056"/>
   </bookViews>
   <sheets>
-    <sheet name="S1" sheetId="1" r:id="rId1"/>
+    <sheet name="S1" sheetId="5" r:id="rId1"/>
     <sheet name="S2" sheetId="2" r:id="rId2"/>
     <sheet name="S3" sheetId="3" r:id="rId3"/>
     <sheet name="S4" sheetId="4" r:id="rId4"/>
+    <sheet name="S5" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="1307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="1378">
   <si>
     <t>Cohort</t>
   </si>
@@ -3948,13 +3949,226 @@
   </si>
   <si>
     <t>INTERVAL circlize plot</t>
+  </si>
+  <si>
+    <t>tbc</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>/data/erimac/VIS/</t>
+  </si>
+  <si>
+    <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>/data/erimac/</t>
+  </si>
+  <si>
+    <t>E.MacDonald.Dunlop@ed.ac.uk</t>
+  </si>
+  <si>
+    <t>erin macdonald</t>
+  </si>
+  <si>
+    <t>population isolate Croatia</t>
+  </si>
+  <si>
+    <t>www.orcades.ed.ac.uk/orcades/</t>
+  </si>
+  <si>
+    <t>/data/erimac/ORCADES/</t>
+  </si>
+  <si>
+    <t>population isolate Orkney</t>
+  </si>
+  <si>
+    <t>/data/jinhua/KORA</t>
+  </si>
+  <si>
+    <t>Helmholz</t>
+  </si>
+  <si>
+    <t>/data/andmala/</t>
+  </si>
+  <si>
+    <t>anders.malarstig@ki.se</t>
+  </si>
+  <si>
+    <t>anders malarstig</t>
+  </si>
+  <si>
+    <t>population study Germany</t>
+  </si>
+  <si>
+    <t>KORA F4</t>
+  </si>
+  <si>
+    <t>/data/jampet/upload-20170920/</t>
+  </si>
+  <si>
+    <t>Cambridge</t>
+  </si>
+  <si>
+    <t>/data/jampet/</t>
+  </si>
+  <si>
+    <t>jp549@medschl.cam.ac.uk</t>
+  </si>
+  <si>
+    <t>james peters</t>
+  </si>
+  <si>
+    <t>blood donors England</t>
+  </si>
+  <si>
+    <t>www.intervalstudy.org.uk/</t>
+  </si>
+  <si>
+    <t>/data/anekal/EGCUT_INF/</t>
+  </si>
+  <si>
+    <t>Tartu</t>
+  </si>
+  <si>
+    <t>/data/anekal/</t>
+  </si>
+  <si>
+    <t>anette.kalnapenkis@gmail.com</t>
+  </si>
+  <si>
+    <t>anette kalnapenkis</t>
+  </si>
+  <si>
+    <t>population study Estonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.geenivaramu.ee/en/access-biobank </t>
+  </si>
+  <si>
+    <t>Estonian Biobank</t>
+  </si>
+  <si>
+    <t>/data/asahed</t>
+  </si>
+  <si>
+    <t>Karolinska</t>
+  </si>
+  <si>
+    <t>awaited</t>
+  </si>
+  <si>
+    <t>rheumatoid</t>
+  </si>
+  <si>
+    <t>COMBINE.RECOMBINE</t>
+  </si>
+  <si>
+    <t>/data/andmala/biofinder_inf</t>
+  </si>
+  <si>
+    <t>dementia</t>
+  </si>
+  <si>
+    <t>/data/andmala/STANLEY_20180911/</t>
+  </si>
+  <si>
+    <t>bipolar, depression</t>
+  </si>
+  <si>
+    <t>STANLEY lah1</t>
+  </si>
+  <si>
+    <t>/data/andmala/STANLEY_20180911/swe6_inf</t>
+  </si>
+  <si>
+    <t>STANLEY swe6</t>
+  </si>
+  <si>
+    <t>/data/niceri/Stability_INF1</t>
+  </si>
+  <si>
+    <t>Uppsala</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>/data/niceri/</t>
+  </si>
+  <si>
+    <t>niclas.eriksson@ucr.uu.se</t>
+  </si>
+  <si>
+    <t>niclas eriksson</t>
+  </si>
+  <si>
+    <t>atherosclerosis</t>
+  </si>
+  <si>
+    <t>/data/andmala/madcam/</t>
+  </si>
+  <si>
+    <t>Pfizer</t>
+  </si>
+  <si>
+    <t>Pfizer.trials</t>
+  </si>
+  <si>
+    <t>/data/stefane/NSPHS_INF/</t>
+  </si>
+  <si>
+    <t>/data/stefane/</t>
+  </si>
+  <si>
+    <t>stefan.enroth@igp.uu.se</t>
+  </si>
+  <si>
+    <t>stefan enroth</t>
+  </si>
+  <si>
+    <t>population study Sweden</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>values.below.llod</t>
+  </si>
+  <si>
+    <t>INF.gwas</t>
+  </si>
+  <si>
+    <t>top.level.dir</t>
+  </si>
+  <si>
+    <t>contact.email</t>
+  </si>
+  <si>
+    <t>contact.name</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3970,13 +4184,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3988,10 +4250,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3999,9 +4262,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4328,1822 +4620,494 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10" style="7" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="7" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="31.109375" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="7" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="27.77734375" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="12.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>1372</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>1371</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>1370</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>1369</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D2" s="10">
+        <v>866</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>1366</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>1365</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>1364</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>1311</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>1354</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D3" s="17">
+        <v>185</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>1322</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>1321</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="9" t="s">
+        <v>1361</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2951</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>1358</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>1357</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>1356</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>1355</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>1354</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D5" s="19">
+        <v>300</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>1322</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>1321</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>1311</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D6" s="10">
+        <v>344</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>1322</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>1321</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>1311</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5">
+      <c r="C7" s="9" t="s">
+        <v>1347</v>
+      </c>
+      <c r="D7" s="17">
         <v>1496</v>
       </c>
-      <c r="D5">
-        <v>1496</v>
-      </c>
-      <c r="E5">
-        <v>1496</v>
-      </c>
-      <c r="F5">
-        <v>1496</v>
-      </c>
-      <c r="G5">
-        <v>1496</v>
-      </c>
-      <c r="H5">
-        <v>1496</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6">
+      <c r="E7" s="8" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>1322</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>1321</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="10" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D8" s="10">
+        <v>860</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>1322</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>1343</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D9" s="10">
+        <v>487</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>1337</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>1336</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>1335</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>1311</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>1334</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D10" s="10">
+        <v>4902</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>1328</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>1311</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>1327</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1050</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>1322</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>1321</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="9" t="s">
+        <v>1320</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D12" s="10">
+        <v>981</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>1313</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>1312</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>1311</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>1310</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6">
-        <v>83</v>
-      </c>
-      <c r="E6">
-        <v>333</v>
-      </c>
-      <c r="F6">
-        <v>834</v>
-      </c>
-      <c r="G6">
-        <v>1522</v>
-      </c>
-      <c r="H6">
-        <v>487.2</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>3.3419999999999999E-3</v>
-      </c>
-      <c r="D7">
-        <v>2.7740999999999998E-2</v>
-      </c>
-      <c r="E7">
-        <v>0.11129699999999999</v>
-      </c>
-      <c r="F7">
-        <v>0.27874300000000002</v>
-      </c>
-      <c r="G7">
-        <v>0.50868999999999998</v>
-      </c>
-      <c r="H7">
-        <v>0.16284999999999999</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>487</v>
-      </c>
-      <c r="D11">
-        <v>487</v>
-      </c>
-      <c r="E11">
-        <v>487</v>
-      </c>
-      <c r="F11">
-        <v>487</v>
-      </c>
-      <c r="G11">
-        <v>487</v>
-      </c>
-      <c r="H11">
-        <v>487</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>33</v>
-      </c>
-      <c r="E12">
-        <v>115</v>
-      </c>
-      <c r="F12">
-        <v>260</v>
-      </c>
-      <c r="G12">
-        <v>487</v>
-      </c>
-      <c r="H12">
-        <v>156.9</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>3.5340000000000003E-2</v>
-      </c>
-      <c r="E13">
-        <v>0.12706999999999999</v>
-      </c>
-      <c r="F13">
-        <v>0.29043000000000002</v>
-      </c>
-      <c r="G13">
-        <v>0.5</v>
-      </c>
-      <c r="H13">
-        <v>0.17205000000000001</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0.34589999999999999</v>
-      </c>
-      <c r="E14">
-        <v>0.68559999999999999</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0.64029999999999998</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>487</v>
-      </c>
-      <c r="D16">
-        <v>487</v>
-      </c>
-      <c r="E16">
-        <v>487</v>
-      </c>
-      <c r="F16">
-        <v>487</v>
-      </c>
-      <c r="G16">
-        <v>487</v>
-      </c>
-      <c r="H16">
-        <v>487</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>0.2001</v>
-      </c>
-      <c r="D17">
-        <v>0.89949999999999997</v>
-      </c>
-      <c r="E17">
-        <v>0.96230000000000004</v>
-      </c>
-      <c r="F17">
-        <v>1.0032000000000001</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <v>0.93440000000000001</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>43058</v>
-      </c>
-      <c r="D21">
-        <v>43059</v>
-      </c>
-      <c r="E21">
-        <v>43059</v>
-      </c>
-      <c r="F21">
-        <v>43059</v>
-      </c>
-      <c r="G21">
-        <v>43060</v>
-      </c>
-      <c r="H21">
-        <v>43059</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>16.75</v>
-      </c>
-      <c r="E22">
-        <v>70.349999999999994</v>
-      </c>
-      <c r="F22">
-        <v>787.35</v>
-      </c>
-      <c r="G22">
-        <v>43060</v>
-      </c>
-      <c r="H22">
-        <v>3759.17</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>1.9450000000000001E-4</v>
-      </c>
-      <c r="E23">
-        <v>8.1689999999999996E-4</v>
-      </c>
-      <c r="F23">
-        <v>9.1426000000000007E-3</v>
-      </c>
-      <c r="G23">
-        <v>0.5</v>
-      </c>
-      <c r="H23">
-        <v>4.36514E-2</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0.10059999999999999</v>
-      </c>
-      <c r="G24">
-        <v>69.5</v>
-      </c>
-      <c r="H24">
-        <v>0.14369999999999999</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25">
-        <v>4.9979999999999997E-2</v>
-      </c>
-      <c r="D25">
-        <v>0.58596999999999999</v>
-      </c>
-      <c r="E25">
-        <v>0.75751999999999997</v>
-      </c>
-      <c r="F25">
-        <v>0.96769000000000005</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>0.75131999999999999</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>4896</v>
-      </c>
-      <c r="D26">
-        <v>4896</v>
-      </c>
-      <c r="E26">
-        <v>4896</v>
-      </c>
-      <c r="F26">
-        <v>4896</v>
-      </c>
-      <c r="G26">
-        <v>4896</v>
-      </c>
-      <c r="H26">
-        <v>4896</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>3.8</v>
-      </c>
-      <c r="F27">
-        <v>28.8</v>
-      </c>
-      <c r="G27">
-        <v>4896</v>
-      </c>
-      <c r="H27">
-        <v>328.5</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>3.881E-4</v>
-      </c>
-      <c r="F28">
-        <v>2.9412000000000002E-3</v>
-      </c>
-      <c r="G28">
-        <v>0.5</v>
-      </c>
-      <c r="H28">
-        <v>3.3543200000000002E-2</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>2.9799999999999999E-5</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>0.91227689999999995</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30">
-        <v>4.9759999999999999E-2</v>
-      </c>
-      <c r="D30">
-        <v>0.68322000000000005</v>
-      </c>
-      <c r="E30">
-        <v>0.94189999999999996</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <v>0.83645000000000003</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34">
-        <v>1064</v>
-      </c>
-      <c r="D34">
-        <v>1064</v>
-      </c>
-      <c r="E34">
-        <v>1064</v>
-      </c>
-      <c r="F34">
-        <v>1064</v>
-      </c>
-      <c r="G34">
-        <v>1064</v>
-      </c>
-      <c r="H34">
-        <v>1064</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>5</v>
-      </c>
-      <c r="G35">
-        <v>2128</v>
-      </c>
-      <c r="H35">
-        <v>125.5</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>1.8799999999999999E-3</v>
-      </c>
-      <c r="G36">
-        <v>0.5</v>
-      </c>
-      <c r="H36">
-        <v>3.6060000000000002E-2</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37">
-        <v>0.91590000000000005</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39">
-        <v>1064</v>
-      </c>
-      <c r="D39">
-        <v>1064</v>
-      </c>
-      <c r="E39">
-        <v>1064</v>
-      </c>
-      <c r="F39">
-        <v>1064</v>
-      </c>
-      <c r="G39">
-        <v>1064</v>
-      </c>
-      <c r="H39">
-        <v>1064</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40">
-        <v>1.0029999999999999</v>
-      </c>
-      <c r="D40">
-        <v>10.945</v>
-      </c>
-      <c r="E40">
-        <v>83.42</v>
-      </c>
-      <c r="F40">
-        <v>436.548</v>
-      </c>
-      <c r="G40">
-        <v>1064</v>
-      </c>
-      <c r="H40">
-        <v>251.917</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41">
-        <v>4.7130000000000002E-4</v>
-      </c>
-      <c r="D41">
-        <v>5.1433E-3</v>
-      </c>
-      <c r="E41">
-        <v>3.9201300000000001E-2</v>
-      </c>
-      <c r="F41">
-        <v>0.20514470000000001</v>
-      </c>
-      <c r="G41">
-        <v>0.5</v>
-      </c>
-      <c r="H41">
-        <v>0.1183821</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0.53890000000000005</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-      <c r="H42">
-        <v>0.76419999999999999</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43">
-        <v>9.835E-4</v>
-      </c>
-      <c r="D43">
-        <v>0.60936199999999996</v>
-      </c>
-      <c r="E43">
-        <v>0.88170599999999999</v>
-      </c>
-      <c r="F43">
-        <v>0.97810900000000001</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="H43">
-        <v>0.77018439999999999</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>2</v>
-      </c>
-      <c r="C47">
-        <v>185</v>
-      </c>
-      <c r="D47">
-        <v>185</v>
-      </c>
-      <c r="E47">
-        <v>185</v>
-      </c>
-      <c r="F47">
-        <v>185</v>
-      </c>
-      <c r="G47">
-        <v>185</v>
-      </c>
-      <c r="H47">
-        <v>185</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>2.7029999999999998E-2</v>
-      </c>
-      <c r="E48">
-        <v>0.11892</v>
-      </c>
-      <c r="F48">
-        <v>0.36757000000000001</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48">
-        <v>0.23330999999999999</v>
-      </c>
-      <c r="I48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="D49">
-        <v>0.85299999999999998</v>
-      </c>
-      <c r="E49">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="F49">
-        <v>0.995</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49">
-        <v>0.89249999999999996</v>
-      </c>
-      <c r="I49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
-        <v>2</v>
-      </c>
-      <c r="C53">
-        <v>866</v>
-      </c>
-      <c r="D53">
-        <v>866</v>
-      </c>
-      <c r="E53">
-        <v>866</v>
-      </c>
-      <c r="F53">
-        <v>866</v>
-      </c>
-      <c r="G53">
-        <v>866</v>
-      </c>
-      <c r="H53">
-        <v>866</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54">
-        <v>1.5020000000000001E-3</v>
-      </c>
-      <c r="D54">
-        <v>9.7940000000000006E-3</v>
-      </c>
-      <c r="E54">
-        <v>5.142E-2</v>
-      </c>
-      <c r="F54">
-        <v>0.20710000000000001</v>
-      </c>
-      <c r="G54">
-        <v>0.5</v>
-      </c>
-      <c r="H54">
-        <v>0.12331499999999999</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>0.21840000000000001</v>
-      </c>
-      <c r="E55">
-        <v>0.68779999999999997</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55">
-        <v>1</v>
-      </c>
-      <c r="H55">
-        <v>0.60929999999999995</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B59" t="s">
-        <v>2</v>
-      </c>
-      <c r="C59">
-        <v>982</v>
-      </c>
-      <c r="D59">
-        <v>982</v>
-      </c>
-      <c r="E59">
-        <v>982</v>
-      </c>
-      <c r="F59">
-        <v>982</v>
-      </c>
-      <c r="G59">
-        <v>982</v>
-      </c>
-      <c r="H59">
-        <v>982</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B60" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-      <c r="D60">
-        <v>11.25</v>
-      </c>
-      <c r="E60">
-        <v>78</v>
-      </c>
-      <c r="F60">
-        <v>390.35</v>
-      </c>
-      <c r="G60">
-        <v>982</v>
-      </c>
-      <c r="H60">
-        <v>229.16</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B61" t="s">
-        <v>3</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="D61">
-        <v>5.7279999999999996E-3</v>
-      </c>
-      <c r="E61">
-        <v>3.9715E-2</v>
-      </c>
-      <c r="F61">
-        <v>0.19875300000000001</v>
-      </c>
-      <c r="G61">
-        <v>0.5</v>
-      </c>
-      <c r="H61">
-        <v>0.116679</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B62" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-      <c r="D62">
-        <v>0.40939999999999999</v>
-      </c>
-      <c r="E62">
-        <v>0.90990000000000004</v>
-      </c>
-      <c r="F62">
-        <v>0.90990000000000004</v>
-      </c>
-      <c r="G62">
-        <v>1</v>
-      </c>
-      <c r="H62">
-        <v>0.71020000000000005</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B63" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63">
-        <v>0.05</v>
-      </c>
-      <c r="D63">
-        <v>0.93</v>
-      </c>
-      <c r="E63">
-        <v>0.98</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="G63">
-        <v>1</v>
-      </c>
-      <c r="H63">
-        <v>0.94</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
-        <v>2</v>
-      </c>
-      <c r="C64">
-        <v>980</v>
-      </c>
-      <c r="D64">
-        <v>980</v>
-      </c>
-      <c r="E64">
-        <v>980</v>
-      </c>
-      <c r="F64">
-        <v>980</v>
-      </c>
-      <c r="G64">
-        <v>980</v>
-      </c>
-      <c r="H64">
-        <v>980</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65">
-        <v>0.4</v>
-      </c>
-      <c r="D65">
-        <v>0.92620000000000002</v>
-      </c>
-      <c r="E65">
-        <v>0.98440000000000005</v>
-      </c>
-      <c r="F65">
-        <v>0.99719999999999998</v>
-      </c>
-      <c r="G65">
-        <v>1</v>
-      </c>
-      <c r="H65">
-        <v>0.94130000000000003</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>46</v>
-      </c>
-      <c r="B67" t="s">
-        <v>29</v>
-      </c>
-      <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="I68" s="3"/>
-    </row>
-    <row r="69" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C69" s="4">
-        <v>404</v>
-      </c>
-      <c r="D69" s="4">
-        <v>438</v>
-      </c>
-      <c r="E69" s="4">
-        <v>444</v>
-      </c>
-      <c r="F69" s="4">
-        <v>447</v>
-      </c>
-      <c r="G69" s="4">
-        <v>448</v>
-      </c>
-      <c r="H69" s="4">
-        <v>441.5</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="4">
-        <v>0</v>
-      </c>
-      <c r="D70" s="4">
-        <v>3.356E-2</v>
-      </c>
-      <c r="E70" s="4">
-        <v>0.1016</v>
-      </c>
-      <c r="F70" s="4">
-        <v>0.25230000000000002</v>
-      </c>
-      <c r="G70" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="H70" s="4">
-        <v>0.15501999999999999</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="4">
-        <v>0.21290000000000001</v>
-      </c>
-      <c r="D71" s="4">
-        <v>0.94810000000000005</v>
-      </c>
-      <c r="E71" s="4">
-        <v>0.97170000000000001</v>
-      </c>
-      <c r="F71" s="4">
-        <v>0.98660000000000003</v>
-      </c>
-      <c r="G71" s="4">
-        <v>1</v>
-      </c>
-      <c r="H71" s="4">
-        <v>0.95550000000000002</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="I72" s="3"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>9</v>
-      </c>
-      <c r="B73" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
-        <v>2</v>
-      </c>
-      <c r="C75">
-        <v>2950</v>
-      </c>
-      <c r="D75">
-        <v>2951</v>
-      </c>
-      <c r="E75">
-        <v>2951</v>
-      </c>
-      <c r="F75">
-        <v>2951</v>
-      </c>
-      <c r="G75">
-        <v>2951</v>
-      </c>
-      <c r="H75">
-        <v>2951</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
-        <v>34</v>
-      </c>
-      <c r="C76">
-        <v>22.98</v>
-      </c>
-      <c r="D76">
-        <v>442.8</v>
-      </c>
-      <c r="E76">
-        <v>980.35</v>
-      </c>
-      <c r="F76">
-        <v>1875.54</v>
-      </c>
-      <c r="G76">
-        <v>2951</v>
-      </c>
-      <c r="H76">
-        <v>1192.56</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77">
-        <v>3.8939999999999999E-3</v>
-      </c>
-      <c r="D77">
-        <v>7.5025999999999995E-2</v>
-      </c>
-      <c r="E77">
-        <v>0.16611000000000001</v>
-      </c>
-      <c r="F77">
-        <v>0.31779000000000002</v>
-      </c>
-      <c r="G77">
-        <v>0.5</v>
-      </c>
-      <c r="H77">
-        <v>0.20206199999999999</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>0.18260000000000001</v>
-      </c>
-      <c r="E78">
-        <v>0.49769999999999998</v>
-      </c>
-      <c r="F78">
-        <v>1.1473</v>
-      </c>
-      <c r="G78">
-        <v>6.6829000000000001</v>
-      </c>
-      <c r="H78">
-        <v>0.86739999999999995</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79">
-        <v>0.36870000000000003</v>
-      </c>
-      <c r="D79">
-        <v>0.91010000000000002</v>
-      </c>
-      <c r="E79">
-        <v>0.98619999999999997</v>
-      </c>
-      <c r="F79">
-        <v>0.99709999999999999</v>
-      </c>
-      <c r="G79">
-        <v>1</v>
-      </c>
-      <c r="H79">
-        <v>0.92879999999999996</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80">
-        <v>2951</v>
-      </c>
-      <c r="D80">
-        <v>2951</v>
-      </c>
-      <c r="E80">
-        <v>2951</v>
-      </c>
-      <c r="F80">
-        <v>2951</v>
-      </c>
-      <c r="G80">
-        <v>2951</v>
-      </c>
-      <c r="H80">
-        <v>2951</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B81" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81">
-        <v>0.40010000000000001</v>
-      </c>
-      <c r="D81">
-        <v>0.91020000000000001</v>
-      </c>
-      <c r="E81">
-        <v>0.98619999999999997</v>
-      </c>
-      <c r="F81">
-        <v>0.99709999999999999</v>
-      </c>
-      <c r="G81">
-        <v>1</v>
-      </c>
-      <c r="H81">
-        <v>0.92879999999999996</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>18</v>
-      </c>
-      <c r="B83" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B85" t="s">
-        <v>2</v>
-      </c>
-      <c r="C85">
-        <v>344</v>
-      </c>
-      <c r="D85">
-        <v>344</v>
-      </c>
-      <c r="E85">
-        <v>344</v>
-      </c>
-      <c r="F85">
-        <v>344</v>
-      </c>
-      <c r="G85">
-        <v>344</v>
-      </c>
-      <c r="H85">
-        <v>344</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B86" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-      <c r="D86">
-        <v>0.79969999999999997</v>
-      </c>
-      <c r="E86">
-        <v>0.93189999999999995</v>
-      </c>
-      <c r="F86">
-        <v>0.9879</v>
-      </c>
-      <c r="G86">
-        <v>2</v>
-      </c>
-      <c r="H86">
-        <v>0.87190000000000001</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>19</v>
-      </c>
-      <c r="B88" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B90" t="s">
-        <v>2</v>
-      </c>
-      <c r="C90">
-        <v>300</v>
-      </c>
-      <c r="D90">
-        <v>300</v>
-      </c>
-      <c r="E90">
-        <v>300</v>
-      </c>
-      <c r="F90">
-        <v>300</v>
-      </c>
-      <c r="G90">
-        <v>300</v>
-      </c>
-      <c r="H90">
-        <v>300</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B91" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91">
-        <v>0</v>
-      </c>
-      <c r="D91">
-        <v>0.85599999999999998</v>
-      </c>
-      <c r="E91">
-        <v>0.95220000000000005</v>
-      </c>
-      <c r="F91">
-        <v>0.99829999999999997</v>
-      </c>
-      <c r="G91">
-        <v>2</v>
-      </c>
-      <c r="H91">
-        <v>0.90029999999999999</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>10</v>
-      </c>
-      <c r="B93" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B95" t="s">
-        <v>2</v>
-      </c>
-      <c r="C95">
-        <v>902</v>
-      </c>
-      <c r="D95">
-        <v>902</v>
-      </c>
-      <c r="E95">
-        <v>902</v>
-      </c>
-      <c r="F95">
-        <v>902</v>
-      </c>
-      <c r="G95">
-        <v>902</v>
-      </c>
-      <c r="H95">
-        <v>902</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B96" t="s">
-        <v>34</v>
-      </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-      <c r="D96">
-        <v>7.85</v>
-      </c>
-      <c r="E96">
-        <v>60.55</v>
-      </c>
-      <c r="F96">
-        <v>338.2</v>
-      </c>
-      <c r="G96">
-        <v>902</v>
-      </c>
-      <c r="H96">
-        <v>201.35</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B97" t="s">
-        <v>3</v>
-      </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
-      <c r="D97">
-        <v>4.3509999999999998E-3</v>
-      </c>
-      <c r="E97">
-        <v>3.3563999999999997E-2</v>
-      </c>
-      <c r="F97">
-        <v>0.187472</v>
-      </c>
-      <c r="G97">
-        <v>0.5</v>
-      </c>
-      <c r="H97">
-        <v>0.111612</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B98" t="s">
-        <v>4</v>
-      </c>
-      <c r="C98">
-        <v>1.9999999999999999E-7</v>
-      </c>
-      <c r="D98">
-        <v>0.46566600000000002</v>
-      </c>
-      <c r="E98">
-        <v>1</v>
-      </c>
-      <c r="F98">
-        <v>1</v>
-      </c>
-      <c r="G98">
-        <v>1</v>
-      </c>
-      <c r="H98">
-        <v>0.73655289999999995</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B99" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="D99">
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="E99">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="F99">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="G99">
-        <v>1</v>
-      </c>
-      <c r="H99">
-        <v>0.85699999999999998</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B100" t="s">
-        <v>2</v>
-      </c>
-      <c r="C100">
-        <v>901</v>
-      </c>
-      <c r="D100">
-        <v>901</v>
-      </c>
-      <c r="E100">
-        <v>901</v>
-      </c>
-      <c r="F100">
-        <v>901</v>
-      </c>
-      <c r="G100">
-        <v>901</v>
-      </c>
-      <c r="H100">
-        <v>901</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B101" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101">
-        <v>0.4</v>
-      </c>
-      <c r="D101">
-        <v>0.77790000000000004</v>
-      </c>
-      <c r="E101">
-        <v>0.91549999999999998</v>
-      </c>
-      <c r="F101">
-        <v>0.9819</v>
-      </c>
-      <c r="G101">
-        <v>1</v>
-      </c>
-      <c r="H101">
-        <v>0.86009999999999998</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="B13" s="9" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D13" s="10">
+        <v>899</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>1313</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>1312</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>1311</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>1310</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10">
+        <f>SUM(D2:D13)</f>
+        <v>15321</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="11" t="s">
+        <v>1307</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30230,7 +29194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -30246,4 +29210,1831 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I101"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1496</v>
+      </c>
+      <c r="D5">
+        <v>1496</v>
+      </c>
+      <c r="E5">
+        <v>1496</v>
+      </c>
+      <c r="F5">
+        <v>1496</v>
+      </c>
+      <c r="G5">
+        <v>1496</v>
+      </c>
+      <c r="H5">
+        <v>1496</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>83</v>
+      </c>
+      <c r="E6">
+        <v>333</v>
+      </c>
+      <c r="F6">
+        <v>834</v>
+      </c>
+      <c r="G6">
+        <v>1522</v>
+      </c>
+      <c r="H6">
+        <v>487.2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3.3419999999999999E-3</v>
+      </c>
+      <c r="D7">
+        <v>2.7740999999999998E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.11129699999999999</v>
+      </c>
+      <c r="F7">
+        <v>0.27874300000000002</v>
+      </c>
+      <c r="G7">
+        <v>0.50868999999999998</v>
+      </c>
+      <c r="H7">
+        <v>0.16284999999999999</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>487</v>
+      </c>
+      <c r="D11">
+        <v>487</v>
+      </c>
+      <c r="E11">
+        <v>487</v>
+      </c>
+      <c r="F11">
+        <v>487</v>
+      </c>
+      <c r="G11">
+        <v>487</v>
+      </c>
+      <c r="H11">
+        <v>487</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>115</v>
+      </c>
+      <c r="F12">
+        <v>260</v>
+      </c>
+      <c r="G12">
+        <v>487</v>
+      </c>
+      <c r="H12">
+        <v>156.9</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>3.5340000000000003E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.12706999999999999</v>
+      </c>
+      <c r="F13">
+        <v>0.29043000000000002</v>
+      </c>
+      <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="H13">
+        <v>0.17205000000000001</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.34589999999999999</v>
+      </c>
+      <c r="E14">
+        <v>0.68559999999999999</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0.64029999999999998</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>487</v>
+      </c>
+      <c r="D16">
+        <v>487</v>
+      </c>
+      <c r="E16">
+        <v>487</v>
+      </c>
+      <c r="F16">
+        <v>487</v>
+      </c>
+      <c r="G16">
+        <v>487</v>
+      </c>
+      <c r="H16">
+        <v>487</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>0.2001</v>
+      </c>
+      <c r="D17">
+        <v>0.89949999999999997</v>
+      </c>
+      <c r="E17">
+        <v>0.96230000000000004</v>
+      </c>
+      <c r="F17">
+        <v>1.0032000000000001</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>0.93440000000000001</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>43058</v>
+      </c>
+      <c r="D21">
+        <v>43059</v>
+      </c>
+      <c r="E21">
+        <v>43059</v>
+      </c>
+      <c r="F21">
+        <v>43059</v>
+      </c>
+      <c r="G21">
+        <v>43060</v>
+      </c>
+      <c r="H21">
+        <v>43059</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>16.75</v>
+      </c>
+      <c r="E22">
+        <v>70.349999999999994</v>
+      </c>
+      <c r="F22">
+        <v>787.35</v>
+      </c>
+      <c r="G22">
+        <v>43060</v>
+      </c>
+      <c r="H22">
+        <v>3759.17</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1.9450000000000001E-4</v>
+      </c>
+      <c r="E23">
+        <v>8.1689999999999996E-4</v>
+      </c>
+      <c r="F23">
+        <v>9.1426000000000007E-3</v>
+      </c>
+      <c r="G23">
+        <v>0.5</v>
+      </c>
+      <c r="H23">
+        <v>4.36514E-2</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0.10059999999999999</v>
+      </c>
+      <c r="G24">
+        <v>69.5</v>
+      </c>
+      <c r="H24">
+        <v>0.14369999999999999</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>4.9979999999999997E-2</v>
+      </c>
+      <c r="D25">
+        <v>0.58596999999999999</v>
+      </c>
+      <c r="E25">
+        <v>0.75751999999999997</v>
+      </c>
+      <c r="F25">
+        <v>0.96769000000000005</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0.75131999999999999</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>4896</v>
+      </c>
+      <c r="D26">
+        <v>4896</v>
+      </c>
+      <c r="E26">
+        <v>4896</v>
+      </c>
+      <c r="F26">
+        <v>4896</v>
+      </c>
+      <c r="G26">
+        <v>4896</v>
+      </c>
+      <c r="H26">
+        <v>4896</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>3.8</v>
+      </c>
+      <c r="F27">
+        <v>28.8</v>
+      </c>
+      <c r="G27">
+        <v>4896</v>
+      </c>
+      <c r="H27">
+        <v>328.5</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>3.881E-4</v>
+      </c>
+      <c r="F28">
+        <v>2.9412000000000002E-3</v>
+      </c>
+      <c r="G28">
+        <v>0.5</v>
+      </c>
+      <c r="H28">
+        <v>3.3543200000000002E-2</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>2.9799999999999999E-5</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0.91227689999999995</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>4.9759999999999999E-2</v>
+      </c>
+      <c r="D30">
+        <v>0.68322000000000005</v>
+      </c>
+      <c r="E30">
+        <v>0.94189999999999996</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0.83645000000000003</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>1064</v>
+      </c>
+      <c r="D34">
+        <v>1064</v>
+      </c>
+      <c r="E34">
+        <v>1064</v>
+      </c>
+      <c r="F34">
+        <v>1064</v>
+      </c>
+      <c r="G34">
+        <v>1064</v>
+      </c>
+      <c r="H34">
+        <v>1064</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>2128</v>
+      </c>
+      <c r="H35">
+        <v>125.5</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1.8799999999999999E-3</v>
+      </c>
+      <c r="G36">
+        <v>0.5</v>
+      </c>
+      <c r="H36">
+        <v>3.6060000000000002E-2</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>0.91590000000000005</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>1064</v>
+      </c>
+      <c r="D39">
+        <v>1064</v>
+      </c>
+      <c r="E39">
+        <v>1064</v>
+      </c>
+      <c r="F39">
+        <v>1064</v>
+      </c>
+      <c r="G39">
+        <v>1064</v>
+      </c>
+      <c r="H39">
+        <v>1064</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="D40">
+        <v>10.945</v>
+      </c>
+      <c r="E40">
+        <v>83.42</v>
+      </c>
+      <c r="F40">
+        <v>436.548</v>
+      </c>
+      <c r="G40">
+        <v>1064</v>
+      </c>
+      <c r="H40">
+        <v>251.917</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>4.7130000000000002E-4</v>
+      </c>
+      <c r="D41">
+        <v>5.1433E-3</v>
+      </c>
+      <c r="E41">
+        <v>3.9201300000000001E-2</v>
+      </c>
+      <c r="F41">
+        <v>0.20514470000000001</v>
+      </c>
+      <c r="G41">
+        <v>0.5</v>
+      </c>
+      <c r="H41">
+        <v>0.1183821</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0.53890000000000005</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>0.76419999999999999</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>9.835E-4</v>
+      </c>
+      <c r="D43">
+        <v>0.60936199999999996</v>
+      </c>
+      <c r="E43">
+        <v>0.88170599999999999</v>
+      </c>
+      <c r="F43">
+        <v>0.97810900000000001</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>0.77018439999999999</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>185</v>
+      </c>
+      <c r="D47">
+        <v>185</v>
+      </c>
+      <c r="E47">
+        <v>185</v>
+      </c>
+      <c r="F47">
+        <v>185</v>
+      </c>
+      <c r="G47">
+        <v>185</v>
+      </c>
+      <c r="H47">
+        <v>185</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>2.7029999999999998E-2</v>
+      </c>
+      <c r="E48">
+        <v>0.11892</v>
+      </c>
+      <c r="F48">
+        <v>0.36757000000000001</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>0.23330999999999999</v>
+      </c>
+      <c r="I48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="D49">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="E49">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="F49">
+        <v>0.995</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>0.89249999999999996</v>
+      </c>
+      <c r="I49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>866</v>
+      </c>
+      <c r="D53">
+        <v>866</v>
+      </c>
+      <c r="E53">
+        <v>866</v>
+      </c>
+      <c r="F53">
+        <v>866</v>
+      </c>
+      <c r="G53">
+        <v>866</v>
+      </c>
+      <c r="H53">
+        <v>866</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>1.5020000000000001E-3</v>
+      </c>
+      <c r="D54">
+        <v>9.7940000000000006E-3</v>
+      </c>
+      <c r="E54">
+        <v>5.142E-2</v>
+      </c>
+      <c r="F54">
+        <v>0.20710000000000001</v>
+      </c>
+      <c r="G54">
+        <v>0.5</v>
+      </c>
+      <c r="H54">
+        <v>0.12331499999999999</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0.21840000000000001</v>
+      </c>
+      <c r="E55">
+        <v>0.68779999999999997</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>0.60929999999999995</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>982</v>
+      </c>
+      <c r="D59">
+        <v>982</v>
+      </c>
+      <c r="E59">
+        <v>982</v>
+      </c>
+      <c r="F59">
+        <v>982</v>
+      </c>
+      <c r="G59">
+        <v>982</v>
+      </c>
+      <c r="H59">
+        <v>982</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>11.25</v>
+      </c>
+      <c r="E60">
+        <v>78</v>
+      </c>
+      <c r="F60">
+        <v>390.35</v>
+      </c>
+      <c r="G60">
+        <v>982</v>
+      </c>
+      <c r="H60">
+        <v>229.16</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>5.7279999999999996E-3</v>
+      </c>
+      <c r="E61">
+        <v>3.9715E-2</v>
+      </c>
+      <c r="F61">
+        <v>0.19875300000000001</v>
+      </c>
+      <c r="G61">
+        <v>0.5</v>
+      </c>
+      <c r="H61">
+        <v>0.116679</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0.40939999999999999</v>
+      </c>
+      <c r="E62">
+        <v>0.90990000000000004</v>
+      </c>
+      <c r="F62">
+        <v>0.90990000000000004</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>0.71020000000000005</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>0.05</v>
+      </c>
+      <c r="D63">
+        <v>0.93</v>
+      </c>
+      <c r="E63">
+        <v>0.98</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>0.94</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>980</v>
+      </c>
+      <c r="D64">
+        <v>980</v>
+      </c>
+      <c r="E64">
+        <v>980</v>
+      </c>
+      <c r="F64">
+        <v>980</v>
+      </c>
+      <c r="G64">
+        <v>980</v>
+      </c>
+      <c r="H64">
+        <v>980</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>0.4</v>
+      </c>
+      <c r="D65">
+        <v>0.92620000000000002</v>
+      </c>
+      <c r="E65">
+        <v>0.98440000000000005</v>
+      </c>
+      <c r="F65">
+        <v>0.99719999999999998</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>0.94130000000000003</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" t="s">
+        <v>29</v>
+      </c>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="4">
+        <v>404</v>
+      </c>
+      <c r="D69" s="4">
+        <v>438</v>
+      </c>
+      <c r="E69" s="4">
+        <v>444</v>
+      </c>
+      <c r="F69" s="4">
+        <v>447</v>
+      </c>
+      <c r="G69" s="4">
+        <v>448</v>
+      </c>
+      <c r="H69" s="4">
+        <v>441.5</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0</v>
+      </c>
+      <c r="D70" s="4">
+        <v>3.356E-2</v>
+      </c>
+      <c r="E70" s="4">
+        <v>0.1016</v>
+      </c>
+      <c r="F70" s="4">
+        <v>0.25230000000000002</v>
+      </c>
+      <c r="G70" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H70" s="4">
+        <v>0.15501999999999999</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0.21290000000000001</v>
+      </c>
+      <c r="D71" s="4">
+        <v>0.94810000000000005</v>
+      </c>
+      <c r="E71" s="4">
+        <v>0.97170000000000001</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0.98660000000000003</v>
+      </c>
+      <c r="G71" s="4">
+        <v>1</v>
+      </c>
+      <c r="H71" s="4">
+        <v>0.95550000000000002</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <v>2950</v>
+      </c>
+      <c r="D75">
+        <v>2951</v>
+      </c>
+      <c r="E75">
+        <v>2951</v>
+      </c>
+      <c r="F75">
+        <v>2951</v>
+      </c>
+      <c r="G75">
+        <v>2951</v>
+      </c>
+      <c r="H75">
+        <v>2951</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76">
+        <v>22.98</v>
+      </c>
+      <c r="D76">
+        <v>442.8</v>
+      </c>
+      <c r="E76">
+        <v>980.35</v>
+      </c>
+      <c r="F76">
+        <v>1875.54</v>
+      </c>
+      <c r="G76">
+        <v>2951</v>
+      </c>
+      <c r="H76">
+        <v>1192.56</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <v>3.8939999999999999E-3</v>
+      </c>
+      <c r="D77">
+        <v>7.5025999999999995E-2</v>
+      </c>
+      <c r="E77">
+        <v>0.16611000000000001</v>
+      </c>
+      <c r="F77">
+        <v>0.31779000000000002</v>
+      </c>
+      <c r="G77">
+        <v>0.5</v>
+      </c>
+      <c r="H77">
+        <v>0.20206199999999999</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0.18260000000000001</v>
+      </c>
+      <c r="E78">
+        <v>0.49769999999999998</v>
+      </c>
+      <c r="F78">
+        <v>1.1473</v>
+      </c>
+      <c r="G78">
+        <v>6.6829000000000001</v>
+      </c>
+      <c r="H78">
+        <v>0.86739999999999995</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <v>0.36870000000000003</v>
+      </c>
+      <c r="D79">
+        <v>0.91010000000000002</v>
+      </c>
+      <c r="E79">
+        <v>0.98619999999999997</v>
+      </c>
+      <c r="F79">
+        <v>0.99709999999999999</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>0.92879999999999996</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80">
+        <v>2951</v>
+      </c>
+      <c r="D80">
+        <v>2951</v>
+      </c>
+      <c r="E80">
+        <v>2951</v>
+      </c>
+      <c r="F80">
+        <v>2951</v>
+      </c>
+      <c r="G80">
+        <v>2951</v>
+      </c>
+      <c r="H80">
+        <v>2951</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81">
+        <v>0.40010000000000001</v>
+      </c>
+      <c r="D81">
+        <v>0.91020000000000001</v>
+      </c>
+      <c r="E81">
+        <v>0.98619999999999997</v>
+      </c>
+      <c r="F81">
+        <v>0.99709999999999999</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>0.92879999999999996</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>2</v>
+      </c>
+      <c r="C85">
+        <v>344</v>
+      </c>
+      <c r="D85">
+        <v>344</v>
+      </c>
+      <c r="E85">
+        <v>344</v>
+      </c>
+      <c r="F85">
+        <v>344</v>
+      </c>
+      <c r="G85">
+        <v>344</v>
+      </c>
+      <c r="H85">
+        <v>344</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0.79969999999999997</v>
+      </c>
+      <c r="E86">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="F86">
+        <v>0.9879</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+      <c r="H86">
+        <v>0.87190000000000001</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <v>300</v>
+      </c>
+      <c r="D90">
+        <v>300</v>
+      </c>
+      <c r="E90">
+        <v>300</v>
+      </c>
+      <c r="F90">
+        <v>300</v>
+      </c>
+      <c r="G90">
+        <v>300</v>
+      </c>
+      <c r="H90">
+        <v>300</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="E91">
+        <v>0.95220000000000005</v>
+      </c>
+      <c r="F91">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="G91">
+        <v>2</v>
+      </c>
+      <c r="H91">
+        <v>0.90029999999999999</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95">
+        <v>902</v>
+      </c>
+      <c r="D95">
+        <v>902</v>
+      </c>
+      <c r="E95">
+        <v>902</v>
+      </c>
+      <c r="F95">
+        <v>902</v>
+      </c>
+      <c r="G95">
+        <v>902</v>
+      </c>
+      <c r="H95">
+        <v>902</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>34</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>7.85</v>
+      </c>
+      <c r="E96">
+        <v>60.55</v>
+      </c>
+      <c r="F96">
+        <v>338.2</v>
+      </c>
+      <c r="G96">
+        <v>902</v>
+      </c>
+      <c r="H96">
+        <v>201.35</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>4.3509999999999998E-3</v>
+      </c>
+      <c r="E97">
+        <v>3.3563999999999997E-2</v>
+      </c>
+      <c r="F97">
+        <v>0.187472</v>
+      </c>
+      <c r="G97">
+        <v>0.5</v>
+      </c>
+      <c r="H97">
+        <v>0.111612</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="D98">
+        <v>0.46566600000000002</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>0.73655289999999995</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D99">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="E99">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="F99">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100">
+        <v>901</v>
+      </c>
+      <c r="D100">
+        <v>901</v>
+      </c>
+      <c r="E100">
+        <v>901</v>
+      </c>
+      <c r="F100">
+        <v>901</v>
+      </c>
+      <c r="G100">
+        <v>901</v>
+      </c>
+      <c r="H100">
+        <v>901</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101">
+        <v>0.4</v>
+      </c>
+      <c r="D101">
+        <v>0.77790000000000004</v>
+      </c>
+      <c r="E101">
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="F101">
+        <v>0.9819</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="H101">
+        <v>0.86009999999999998</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>